<commit_message>
nuevo diseño mas preparacion para aws
</commit_message>
<xml_diff>
--- a/data/PEAJE_PASE_2025.xlsx
+++ b/data/PEAJE_PASE_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo 1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo 1\Desktop\Araiza_Intelligence-Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C94DA4-F4D5-4670-9AED-36111E70DCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFF242-F9B5-4E5B-BEFC-EE7AA3456F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3619,6 +3619,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3647,20 +3661,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3675,12 +3675,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8C44106-EEAF-4E6A-AE1E-1C1ECB9ED605}" name="Tabla1" displayName="Tabla1" ref="A1:R1007" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8C44106-EEAF-4E6A-AE1E-1C1ECB9ED605}" name="Tabla1" displayName="Tabla1" ref="A1:R1007" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:R1007" xr:uid="{B8C44106-EEAF-4E6A-AE1E-1C1ECB9ED605}">
     <filterColumn colId="2">
       <filters>
-        <filter val="JUAREZ-LINCOLN"/>
-        <filter val="LINCOLN"/>
+        <filter val="S. MARTIN PUE"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3997,14 +3996,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M172" sqref="M172"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C474" sqref="C474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" customWidth="1"/>
@@ -13157,7 +13157,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>180</v>
       </c>
@@ -29529,7 +29529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="474" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>155</v>
       </c>
@@ -30177,7 +30177,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="486" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>434</v>
       </c>

</xml_diff>